<commit_message>
fix crane base rates
</commit_message>
<xml_diff>
--- a/data/crane-base-rates.xlsx
+++ b/data/crane-base-rates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hff/Desktop/haarhoff-diss/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE22FC1-741A-A247-8003-BE7C09999CBC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD350447-726A-2D40-BC8E-0CD188562950}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -666,7 +666,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -678,7 +678,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -718,11 +718,11 @@
   </autoFilter>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{137D5F84-EADF-2C4E-A8F5-20E1C53FC8AC}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{E7396C05-1890-AE42-B656-1B2B736881A2}" name="Height [m]" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{39218ECF-A94C-9E4E-8EB8-7CE1CA3F3240}" name="Reach [m]" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{2D061BA1-9763-4845-B0C2-1B49C02FADAE}" name="max Load [kg]" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{10766B31-3A11-6E42-8E19-5F40758C890F}" name="max Load at Tip [kg]" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{EA8BC229-3F0A-C247-A071-E95CE1FA5CD5}" name="Translational Speed [m/min]" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{E7396C05-1890-AE42-B656-1B2B736881A2}" name="Height [m]" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{39218ECF-A94C-9E4E-8EB8-7CE1CA3F3240}" name="Reach [m]" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{2D061BA1-9763-4845-B0C2-1B49C02FADAE}" name="max Load [kg]" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{10766B31-3A11-6E42-8E19-5F40758C890F}" name="max Load at Tip [kg]" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{EA8BC229-3F0A-C247-A071-E95CE1FA5CD5}" name="Translational Speed [m/min]" dataDxfId="8"/>
     <tableColumn id="7" xr3:uid="{F45A958E-7A83-614D-BF77-855E40419EFA}" name="Rotational Speed [rpm]" dataDxfId="7"/>
     <tableColumn id="8" xr3:uid="{214973FB-0D8C-2547-979D-534543D2DD2E}" name="v_trolley" dataDxfId="6">
       <calculatedColumnFormula>Table1[[#This Row],[Translational Speed '[m/min']]]/60</calculatedColumnFormula>
@@ -731,10 +731,10 @@
       <calculatedColumnFormula>Table1[[#This Row],[Rotational Speed '[rpm']]]*2*3.141*Table1[[#This Row],[Reach '[m']]] / 60</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{F8F09299-003D-2341-AAE8-D7AD99D7587A}" name="omega_t" dataDxfId="1">
-      <calculatedColumnFormula>Table1[[#This Row],[v_trolley]] / Table1[[#This Row],[Height '[m']]]</calculatedColumnFormula>
+      <calculatedColumnFormula>Table1[[#This Row],[v_trolley]] * Table1[[#This Row],[Height '[m']]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{09AFA325-0618-7447-BAD1-D939A2CF5A67}" name="omega_j" dataDxfId="0">
-      <calculatedColumnFormula>Table1[[#This Row],[v_jib]] / Table1[[#This Row],[Height '[m']]]</calculatedColumnFormula>
+      <calculatedColumnFormula>Table1[[#This Row],[v_jib]] * Table1[[#This Row],[Height '[m']]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{6374AB4B-A0E0-CE4D-BB89-0E81971B8C74}" name="h_max_t" dataDxfId="4">
       <calculatedColumnFormula>(Table1[[#This Row],[max Load '[kg']]]*Table1[[#This Row],[v_trolley]]*Table1[[#This Row],[v_trolley]]) / (2 * Table1[[#This Row],[max Load '[kg']]] * 9.81)</calculatedColumnFormula>
@@ -1050,19 +1050,19 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N5"/>
+      <selection activeCell="J2" sqref="J2:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="9.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="13" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="18.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="25.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="20.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="13" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="25.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
@@ -1150,12 +1150,12 @@
         <v>1.3087500000000001</v>
       </c>
       <c r="J2" s="3">
-        <f>Table1[[#This Row],[v_trolley]] / Table1[[#This Row],[Height '[m']]]</f>
-        <v>1.9298245614035085E-2</v>
+        <f>Table1[[#This Row],[v_trolley]] * Table1[[#This Row],[Height '[m']]]</f>
+        <v>6.9666666666666659</v>
       </c>
       <c r="K2" s="3">
-        <f>Table1[[#This Row],[v_jib]] / Table1[[#This Row],[Height '[m']]]</f>
-        <v>6.8881578947368419E-2</v>
+        <f>Table1[[#This Row],[v_jib]] * Table1[[#This Row],[Height '[m']]]</f>
+        <v>24.866250000000001</v>
       </c>
       <c r="L2" s="3">
         <f>(Table1[[#This Row],[max Load '[kg']]]*Table1[[#This Row],[v_trolley]]*Table1[[#This Row],[v_trolley]]) / (2 * Table1[[#This Row],[max Load '[kg']]] * 9.81)</f>
@@ -1201,12 +1201,12 @@
         <v>4.1880000000000006</v>
       </c>
       <c r="J3" s="3">
-        <f>Table1[[#This Row],[v_trolley]] / Table1[[#This Row],[Height '[m']]]</f>
-        <v>2.3333333333333334E-2</v>
+        <f>Table1[[#This Row],[v_trolley]] * Table1[[#This Row],[Height '[m']]]</f>
+        <v>47.25</v>
       </c>
       <c r="K3" s="3">
-        <f>Table1[[#This Row],[v_jib]] / Table1[[#This Row],[Height '[m']]]</f>
-        <v>9.3066666666666686E-2</v>
+        <f>Table1[[#This Row],[v_jib]] * Table1[[#This Row],[Height '[m']]]</f>
+        <v>188.46000000000004</v>
       </c>
       <c r="L3" s="3">
         <f>(Table1[[#This Row],[max Load '[kg']]]*Table1[[#This Row],[v_trolley]]*Table1[[#This Row],[v_trolley]]) / (2 * Table1[[#This Row],[max Load '[kg']]] * 9.81)</f>
@@ -1252,12 +1252,12 @@
         <v>6.2820000000000009</v>
       </c>
       <c r="J4" s="3">
-        <f>Table1[[#This Row],[v_trolley]] / Table1[[#This Row],[Height '[m']]]</f>
-        <v>1.9076305220883532E-2</v>
+        <f>Table1[[#This Row],[v_trolley]] * Table1[[#This Row],[Height '[m']]]</f>
+        <v>131.41666666666666</v>
       </c>
       <c r="K4" s="3">
-        <f>Table1[[#This Row],[v_jib]] / Table1[[#This Row],[Height '[m']]]</f>
-        <v>7.5686746987951817E-2</v>
+        <f>Table1[[#This Row],[v_jib]] * Table1[[#This Row],[Height '[m']]]</f>
+        <v>521.40600000000006</v>
       </c>
       <c r="L4" s="3">
         <f>(Table1[[#This Row],[max Load '[kg']]]*Table1[[#This Row],[v_trolley]]*Table1[[#This Row],[v_trolley]]) / (2 * Table1[[#This Row],[max Load '[kg']]] * 9.81)</f>
@@ -1303,12 +1303,12 @@
         <v>2.2929299999999997</v>
       </c>
       <c r="J5" s="3">
-        <f>Table1[[#This Row],[v_trolley]] / Table1[[#This Row],[Height '[m']]]</f>
-        <v>1.7361111111111112E-2</v>
+        <f>Table1[[#This Row],[v_trolley]] * Table1[[#This Row],[Height '[m']]]</f>
+        <v>160</v>
       </c>
       <c r="K5" s="3">
-        <f>Table1[[#This Row],[v_jib]] / Table1[[#This Row],[Height '[m']]]</f>
-        <v>2.3884687499999998E-2</v>
+        <f>Table1[[#This Row],[v_jib]] * Table1[[#This Row],[Height '[m']]]</f>
+        <v>220.12127999999996</v>
       </c>
       <c r="L5" s="3">
         <f>(Table1[[#This Row],[max Load '[kg']]]*Table1[[#This Row],[v_trolley]]*Table1[[#This Row],[v_trolley]]) / (2 * Table1[[#This Row],[max Load '[kg']]] * 9.81)</f>

</xml_diff>